<commit_message>
added Google Maps api and current location
</commit_message>
<xml_diff>
--- a/project2_tennis_pt_app.xlsx
+++ b/project2_tennis_pt_app.xlsx
@@ -2912,7 +2912,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="228">
+  <cellStyleXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3094,6 +3094,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3601,7 +3637,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
-  <cellStyles count="228">
+  <cellStyles count="264">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3727,6 +3763,24 @@
     <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3829,6 +3883,24 @@
     <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5044,7 +5116,7 @@
       <pane xSplit="1" ySplit="18" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9:Z9"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11:Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>